<commit_message>
fixed student processing bug and updated import.xlsx
</commit_message>
<xml_diff>
--- a/import.xlsx
+++ b/import.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\kaart\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="20010" windowHeight="8025"/>
   </bookViews>
@@ -66,9 +61,6 @@
     <t>Opdracht_type</t>
   </si>
   <si>
-    <t>O0003</t>
-  </si>
-  <si>
     <t>Avans Hogeschool 's-Hertogenbosch</t>
   </si>
   <si>
@@ -220,13 +212,16 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>O0002</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,7 +268,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -289,9 +284,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -329,9 +324,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -363,10 +358,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -398,10 +392,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -574,19 +567,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:R23"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -600,31 +593,31 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -638,66 +631,66 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H2">
         <v>17</v>
       </c>
       <c r="I2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
         <v>65</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="C3" t="s">
         <v>36</v>
       </c>
-      <c r="K2" t="s">
-        <v>40</v>
-      </c>
-      <c r="L2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>37</v>
       </c>
-      <c r="D3" t="s">
-        <v>38</v>
-      </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3">
         <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -710,14 +703,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:Q37"/>
+      <selection activeCell="A3" sqref="A3:AC264"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.42578125" customWidth="1"/>
@@ -733,7 +726,7 @@
     <col min="12" max="12" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -741,7 +734,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -750,36 +743,36 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D2" s="2">
         <v>51689155</v>
@@ -788,25 +781,25 @@
         <v>5287245</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H2">
         <v>215</v>
       </c>
       <c r="I2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="K2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -818,14 +811,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:J28"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.140625" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
@@ -835,32 +828,32 @@
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
         <v>8</v>
       </c>
       <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
         <v>45</v>
-      </c>
-      <c r="E1" t="s">
-        <v>46</v>
       </c>
       <c r="F1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -872,15 +865,15 @@
         <v>41365</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -892,7 +885,7 @@
         <v>41579</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -901,14 +894,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:K17"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.140625" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
@@ -918,38 +911,38 @@
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
       <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s">
         <v>57</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>58</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>59</v>
       </c>
-      <c r="G1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -964,15 +957,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3">
         <v>5</v>

</xml_diff>